<commit_message>
added requirement.txt and made changes to the dashboard
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
@@ -522,350 +522,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Daniel Korley</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>JHS 3</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>04/15/1995</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Christian</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>David Korley</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Patience Afari Agyei</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Politician</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Prince Korley</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>JHS 3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>03/16/1990</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Hindu</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Electronics</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>David Korley</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Patience Afari</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Politician</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Sandra Anderson</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>PRIMARY 1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>02/14/2023</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>hindu</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>David</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>lydia</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>business</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>trader</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Dinah Anderson</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>PRIMARY 4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>02/07/2023</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Hindu</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>IT</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>lydia</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>mason</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>business</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>PRIMARY 3</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>kwame</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>PRIMARY 2</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>02/08/2023</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>02/24/2023</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>bb</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>gffc</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>bbvb</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>bcbc</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>bcbc</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>bbcbcbv</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>